<commit_message>
Onedrive does not like Github
</commit_message>
<xml_diff>
--- a/Data/Human Voluntary Data.xlsx
+++ b/Data/Human Voluntary Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\OneDrive - University of Tennessee\VPC\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveutk-my.sharepoint.com/personal/jweave49_uthsc_edu/Documents/VPC/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D4F087-91DD-436D-9737-5D44B12A759D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{78D4F087-91DD-436D-9737-5D44B12A759D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68B48B6C-64B0-4270-9742-AE1F33198D1D}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-2490" windowWidth="16440" windowHeight="29040" xr2:uid="{BB102C53-C3E1-4D54-83D1-542FA604C574}"/>
+    <workbookView xWindow="-16320" yWindow="-1920" windowWidth="16440" windowHeight="29040" xr2:uid="{BB102C53-C3E1-4D54-83D1-542FA604C574}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5080" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5080" uniqueCount="85">
   <si>
     <t>State</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>DAY</t>
+  </si>
+  <si>
+    <t>1E3-7 H1N1</t>
   </si>
 </sst>
 </file>
@@ -794,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D77C534B-1212-4161-8C68-A242F4FEFD13}">
   <dimension ref="A1:S458"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="G276" workbookViewId="0">
+      <selection activeCell="O329" sqref="O329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17343,7 +17346,7 @@
         <v>22</v>
       </c>
       <c r="O319" s="5" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="P319" s="5" t="s">
         <v>53</v>
@@ -17394,8 +17397,8 @@
       <c r="N320" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O320" s="8" t="s">
-        <v>23</v>
+      <c r="O320" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="P320" s="8" t="s">
         <v>53</v>
@@ -17446,8 +17449,8 @@
       <c r="N321" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O321" s="8" t="s">
-        <v>23</v>
+      <c r="O321" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="P321" s="8" t="s">
         <v>53</v>
@@ -17499,7 +17502,7 @@
         <v>22</v>
       </c>
       <c r="O322" s="5" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="P322" s="5" t="s">
         <v>53</v>
@@ -17551,7 +17554,7 @@
         <v>22</v>
       </c>
       <c r="O323" s="5" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="P323" s="5" t="s">
         <v>53</v>
@@ -17603,7 +17606,7 @@
         <v>22</v>
       </c>
       <c r="O324" s="5" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="P324" s="5" t="s">
         <v>53</v>
@@ -17654,8 +17657,8 @@
       <c r="N325" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O325" s="8" t="s">
-        <v>23</v>
+      <c r="O325" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="P325" s="8" t="s">
         <v>53</v>
@@ -17706,8 +17709,8 @@
       <c r="N326" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O326" s="8" t="s">
-        <v>23</v>
+      <c r="O326" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="P326" s="8" t="s">
         <v>53</v>
@@ -17759,7 +17762,7 @@
         <v>22</v>
       </c>
       <c r="O327" s="5" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="P327" s="5" t="s">
         <v>53</v>
@@ -17810,8 +17813,8 @@
       <c r="N328" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O328" s="8" t="s">
-        <v>23</v>
+      <c r="O328" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="P328" s="8" t="s">
         <v>53</v>

</xml_diff>